<commit_message>
updated text to free range
</commit_message>
<xml_diff>
--- a/new7.xlsx
+++ b/new7.xlsx
@@ -6698,10 +6698,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="6" max="6" width="53.77734375" customWidth="1"/>
+    <col min="7" max="7" width="45.21875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
+    <col min="9" max="9" width="29.44140625" customWidth="1"/>
+    <col min="10" max="10" width="30.109375" customWidth="1"/>
+    <col min="11" max="11" width="31.5546875" customWidth="1"/>
+    <col min="12" max="12" width="41" customWidth="1"/>
+    <col min="13" max="13" width="46.5546875" customWidth="1"/>
     <col min="14" max="14" width="91" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>